<commit_message>
form chính, dăng nhập
</commit_message>
<xml_diff>
--- a/Phân công công việc phần mềm quản lý khách sạn.xlsx
+++ b/Phân công công việc phần mềm quản lý khách sạn.xlsx
@@ -27,9 +27,6 @@
     <t>Quân</t>
   </si>
   <si>
-    <t>Thiết kế giao diện cửa sổ chính (màn hình đăng nhập, các menu trỏ đến các module con,…). Xây dựng module quản lý người dùng</t>
-  </si>
-  <si>
     <t>Thảo</t>
   </si>
   <si>
@@ -76,6 +73,9 @@
   </si>
   <si>
     <t>Chức</t>
+  </si>
+  <si>
+    <t>Ghép nối các form</t>
   </si>
 </sst>
 </file>
@@ -520,7 +520,7 @@
   <dimension ref="C2:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,81 +538,81 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="3:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
-        <v>4</v>
-      </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C5" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="3:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6" t="s">
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C7" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C8" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="3:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C10" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" t="s">
         <v>2</v>
@@ -620,46 +620,46 @@
     </row>
     <row r="11" spans="3:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C11" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="3:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="3:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C13" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="3:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "form chính, dăng nhập"
This reverts commit 438b93729ca64007f39eb0dab65493dd4e76b9df.
</commit_message>
<xml_diff>
--- a/Phân công công việc phần mềm quản lý khách sạn.xlsx
+++ b/Phân công công việc phần mềm quản lý khách sạn.xlsx
@@ -27,6 +27,9 @@
     <t>Quân</t>
   </si>
   <si>
+    <t>Thiết kế giao diện cửa sổ chính (màn hình đăng nhập, các menu trỏ đến các module con,…). Xây dựng module quản lý người dùng</t>
+  </si>
+  <si>
     <t>Thảo</t>
   </si>
   <si>
@@ -73,9 +76,6 @@
   </si>
   <si>
     <t>Chức</t>
-  </si>
-  <si>
-    <t>Ghép nối các form</t>
   </si>
 </sst>
 </file>
@@ -520,7 +520,7 @@
   <dimension ref="C2:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,81 +538,81 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="3:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="3" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C5" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="3:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C7" s="6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C8" s="7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="3:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C10" s="9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D10" t="s">
         <v>2</v>
@@ -620,46 +620,46 @@
     </row>
     <row r="11" spans="3:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C11" s="10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="3:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="3:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C13" s="12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="3:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>